<commit_message>
published state of ETDataset on 28th of June 2019 - 2
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/crude_oil.carrier.xlsx
+++ b/carriers_source_analyses/crude_oil.carrier.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/carriers_source_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E9910-A1C5-CE4A-9803-D167611CD42D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="4"/>
+    <workbookView xWindow="9960" yWindow="3720" windowWidth="33800" windowHeight="22320" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -52,10 +53,16 @@
     <definedName name="WP_to_MWp" localSheetId="6">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -65,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
   <si>
     <t>Source</t>
   </si>
@@ -442,11 +449,20 @@
   <si>
     <t>https://www.ecb.europa.eu/stats/policy_and_exchange_rates/euro_reference_exchange_rates/html/eurofxref-graph-usd.en.html</t>
   </si>
+  <si>
+    <t>RVO</t>
+  </si>
+  <si>
+    <t>https://www.rvo.nl/file/nederlandse-lijst-van-energiedragers-en-standaard-co2-emissiefactoren-2017pdf</t>
+  </si>
+  <si>
+    <t>source: RVO (see below)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -457,7 +473,7 @@
     <numFmt numFmtId="170" formatCode="0.00000000000"/>
     <numFmt numFmtId="171" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="38">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,6 +625,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -616,6 +633,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -623,6 +641,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -630,6 +649,7 @@
       <sz val="16"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -637,17 +657,20 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -661,11 +684,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -689,6 +714,7 @@
       <sz val="16"/>
       <color rgb="FF474747"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1747,7 +1773,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="345">
-    <cellStyle name="Excel Built-in Normal" xfId="338"/>
+    <cellStyle name="Excel Built-in Normal" xfId="338" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2099,6 +2125,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2120,7 +2149,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 1"/>
+        <xdr:cNvPr id="7" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -2167,7 +2202,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2182,6 +2223,50 @@
         <a:xfrm>
           <a:off x="8585200" y="92062300"/>
           <a:ext cx="13144500" cy="10477500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>235234</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7412D594-60BE-7744-9AE0-9F532C164B84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8686800" y="8585200"/>
+          <a:ext cx="10738134" cy="3492500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2627,13 +2712,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.5" style="31" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="23" customWidth="1"/>
@@ -2642,24 +2727,24 @@
     <col min="5" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="29" customFormat="1">
       <c r="A1" s="27"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="21">
       <c r="A2" s="7"/>
       <c r="B2" s="30" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="30"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="7"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>80</v>
@@ -2668,7 +2753,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="7"/>
       <c r="B5" s="10" t="s">
         <v>14</v>
@@ -2677,7 +2762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="7"/>
       <c r="B6" s="12" t="s">
         <v>9</v>
@@ -2686,17 +2771,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="7"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="7"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="7"/>
       <c r="B9" s="88" t="s">
         <v>15</v>
@@ -2704,13 +2789,13 @@
       <c r="C9" s="89"/>
       <c r="D9" s="156"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="7"/>
       <c r="B10" s="90"/>
       <c r="C10" s="91"/>
       <c r="D10" s="157"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="7"/>
       <c r="B11" s="90" t="s">
         <v>16</v>
@@ -2720,7 +2805,7 @@
       </c>
       <c r="D11" s="157"/>
     </row>
-    <row r="12" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="17" thickBot="1">
       <c r="A12" s="7"/>
       <c r="B12" s="90"/>
       <c r="C12" s="20" t="s">
@@ -2728,7 +2813,7 @@
       </c>
       <c r="D12" s="157"/>
     </row>
-    <row r="13" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="17" thickBot="1">
       <c r="A13" s="7"/>
       <c r="B13" s="90"/>
       <c r="C13" s="93" t="s">
@@ -2736,7 +2821,7 @@
       </c>
       <c r="D13" s="157"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="7"/>
       <c r="B14" s="90"/>
       <c r="C14" s="91" t="s">
@@ -2744,13 +2829,13 @@
       </c>
       <c r="D14" s="157"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="7"/>
       <c r="B15" s="90"/>
       <c r="C15" s="91"/>
       <c r="D15" s="157"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="7"/>
       <c r="B16" s="90" t="s">
         <v>21</v>
@@ -2760,7 +2845,7 @@
       </c>
       <c r="D16" s="157"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="7"/>
       <c r="B17" s="90"/>
       <c r="C17" s="95" t="s">
@@ -2768,7 +2853,7 @@
       </c>
       <c r="D17" s="157"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="7"/>
       <c r="B18" s="90"/>
       <c r="C18" s="96" t="s">
@@ -2776,7 +2861,7 @@
       </c>
       <c r="D18" s="157"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="7"/>
       <c r="B19" s="90"/>
       <c r="C19" s="97" t="s">
@@ -2784,7 +2869,7 @@
       </c>
       <c r="D19" s="157"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="7"/>
       <c r="B20" s="98"/>
       <c r="C20" s="99" t="s">
@@ -2792,7 +2877,7 @@
       </c>
       <c r="D20" s="157"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="7"/>
       <c r="B21" s="98"/>
       <c r="C21" s="100" t="s">
@@ -2800,7 +2885,7 @@
       </c>
       <c r="D21" s="157"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="7"/>
       <c r="B22" s="98"/>
       <c r="C22" s="101" t="s">
@@ -2808,14 +2893,14 @@
       </c>
       <c r="D22" s="157"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="B23" s="98"/>
       <c r="C23" s="102" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="157"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="B24" s="158"/>
       <c r="C24" s="159"/>
       <c r="D24" s="160"/>
@@ -2827,8 +2912,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="B1:J15"/>
@@ -2837,7 +2922,7 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="38" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="38" customWidth="1"/>
@@ -2852,13 +2937,13 @@
     <col min="11" max="16384" width="10.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10">
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="183" t="s">
         <v>108</v>
       </c>
@@ -2868,7 +2953,7 @@
       <c r="F2" s="184"/>
       <c r="G2" s="185"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10">
       <c r="B3" s="186"/>
       <c r="C3" s="187"/>
       <c r="D3" s="187"/>
@@ -2876,7 +2961,7 @@
       <c r="F3" s="187"/>
       <c r="G3" s="188"/>
     </row>
-    <row r="4" spans="2:10" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="76" customHeight="1">
       <c r="B4" s="189"/>
       <c r="C4" s="190"/>
       <c r="D4" s="190"/>
@@ -2884,10 +2969,10 @@
       <c r="F4" s="190"/>
       <c r="G4" s="191"/>
     </row>
-    <row r="5" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="17" thickBot="1">
       <c r="D5" s="36"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="39"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -2898,7 +2983,7 @@
       <c r="I6" s="22"/>
       <c r="J6" s="40"/>
     </row>
-    <row r="7" spans="2:10" s="45" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" s="45" customFormat="1" ht="19">
       <c r="B7" s="103"/>
       <c r="C7" s="21" t="s">
         <v>13</v>
@@ -2919,7 +3004,7 @@
       </c>
       <c r="J7" s="107"/>
     </row>
-    <row r="8" spans="2:10" s="45" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" s="45" customFormat="1" ht="19">
       <c r="B8" s="25"/>
       <c r="C8" s="20"/>
       <c r="D8" s="33"/>
@@ -2930,7 +3015,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="46"/>
     </row>
-    <row r="9" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="25"/>
       <c r="C9" s="155" t="s">
         <v>83</v>
@@ -2943,7 +3028,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="46"/>
     </row>
-    <row r="10" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B10" s="25"/>
       <c r="C10" s="113" t="s">
         <v>38</v>
@@ -2965,7 +3050,7 @@
       </c>
       <c r="J10" s="46"/>
     </row>
-    <row r="11" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B11" s="25"/>
       <c r="C11" s="122" t="s">
         <v>39</v>
@@ -2985,7 +3070,7 @@
       </c>
       <c r="J11" s="46"/>
     </row>
-    <row r="12" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B12" s="25"/>
       <c r="C12" s="122" t="s">
         <v>82</v>
@@ -3005,7 +3090,7 @@
       </c>
       <c r="J12" s="46"/>
     </row>
-    <row r="13" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B13" s="25"/>
       <c r="C13" s="172" t="s">
         <v>105</v>
@@ -3025,7 +3110,7 @@
       </c>
       <c r="J13" s="46"/>
     </row>
-    <row r="14" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B14" s="25"/>
       <c r="C14" s="37" t="s">
         <v>40</v>
@@ -3035,7 +3120,7 @@
       </c>
       <c r="E14" s="115">
         <f>'Research data'!G10</f>
-        <v>7.5499999999999998E-2</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="122"/>
@@ -3045,7 +3130,7 @@
       </c>
       <c r="J14" s="46"/>
     </row>
-    <row r="15" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="20" customHeight="1" thickBot="1">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="43"/>
@@ -3066,8 +3151,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="B1:J19"/>
@@ -3076,7 +3161,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="38" customWidth="1"/>
     <col min="2" max="2" width="3.6640625" style="38" customWidth="1"/>
@@ -3091,13 +3176,13 @@
     <col min="11" max="16384" width="10.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10">
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
     </row>
-    <row r="2" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" ht="15" customHeight="1">
       <c r="B2" s="183" t="s">
         <v>84</v>
       </c>
@@ -3107,7 +3192,7 @@
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10">
       <c r="B3" s="186"/>
       <c r="C3" s="187"/>
       <c r="D3" s="187"/>
@@ -3115,7 +3200,7 @@
       <c r="F3" s="36"/>
       <c r="G3" s="154"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="B4" s="194"/>
       <c r="C4" s="195"/>
       <c r="D4" s="195"/>
@@ -3123,10 +3208,10 @@
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
-    <row r="5" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="17" thickBot="1">
       <c r="D5" s="36"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="39"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -3137,7 +3222,7 @@
       <c r="I6" s="22"/>
       <c r="J6" s="40"/>
     </row>
-    <row r="7" spans="2:10" s="45" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" s="45" customFormat="1" ht="19">
       <c r="B7" s="103"/>
       <c r="C7" s="21" t="s">
         <v>13</v>
@@ -3158,7 +3243,7 @@
       </c>
       <c r="J7" s="107"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10">
       <c r="B8" s="41"/>
       <c r="C8" s="81"/>
       <c r="D8" s="105"/>
@@ -3169,7 +3254,7 @@
       <c r="I8" s="36"/>
       <c r="J8" s="108"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="B9" s="41"/>
       <c r="C9" s="20" t="s">
         <v>37</v>
@@ -3182,7 +3267,7 @@
       <c r="I9" s="36"/>
       <c r="J9" s="108"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="B10" s="41"/>
       <c r="C10" s="20"/>
       <c r="D10" s="105"/>
@@ -3193,7 +3278,7 @@
       <c r="I10" s="36"/>
       <c r="J10" s="108"/>
     </row>
-    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="17" thickBot="1">
       <c r="B11" s="41"/>
       <c r="C11" s="175" t="s">
         <v>106</v>
@@ -3206,7 +3291,7 @@
       <c r="I11" s="122"/>
       <c r="J11" s="108"/>
     </row>
-    <row r="12" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="17" thickBot="1">
       <c r="B12" s="41"/>
       <c r="C12" s="176" t="s">
         <v>43</v>
@@ -3228,7 +3313,7 @@
       </c>
       <c r="J12" s="108"/>
     </row>
-    <row r="13" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="17" thickBot="1">
       <c r="B13" s="41"/>
       <c r="C13" s="176" t="s">
         <v>44</v>
@@ -3250,7 +3335,7 @@
       </c>
       <c r="J13" s="108"/>
     </row>
-    <row r="14" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="17" thickBot="1">
       <c r="B14" s="41"/>
       <c r="C14" s="176" t="s">
         <v>47</v>
@@ -3272,7 +3357,7 @@
       </c>
       <c r="J14" s="108"/>
     </row>
-    <row r="15" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="17" thickBot="1">
       <c r="B15" s="41"/>
       <c r="C15" s="176" t="s">
         <v>46</v>
@@ -3294,7 +3379,7 @@
       </c>
       <c r="J15" s="108"/>
     </row>
-    <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="17" thickBot="1">
       <c r="B16" s="41"/>
       <c r="C16" s="176" t="s">
         <v>40</v>
@@ -3316,7 +3401,7 @@
       </c>
       <c r="J16" s="108"/>
     </row>
-    <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="17" thickBot="1">
       <c r="B17" s="41"/>
       <c r="C17" s="176" t="s">
         <v>45</v>
@@ -3338,7 +3423,7 @@
       </c>
       <c r="J17" s="108"/>
     </row>
-    <row r="18" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="17" thickBot="1">
       <c r="B18" s="41"/>
       <c r="C18" s="177" t="s">
         <v>107</v>
@@ -3357,7 +3442,7 @@
       </c>
       <c r="J18" s="108"/>
     </row>
-    <row r="19" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="20" customHeight="1" thickBot="1">
       <c r="B19" s="42"/>
       <c r="C19" s="43"/>
       <c r="D19" s="43"/>
@@ -3379,8 +3464,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet3">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B1:O25"/>
@@ -3389,7 +3474,7 @@
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="3.5" style="67" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="67" customWidth="1"/>
@@ -3408,8 +3493,8 @@
     <col min="16" max="16384" width="10.83203125" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" ht="17" thickBot="1"/>
+    <row r="2" spans="2:15">
       <c r="B2" s="69"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -3425,7 +3510,7 @@
       <c r="N2" s="71"/>
       <c r="O2" s="72"/>
     </row>
-    <row r="3" spans="2:15" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" s="26" customFormat="1">
       <c r="B3" s="25"/>
       <c r="C3" s="112" t="s">
         <v>30</v>
@@ -3455,7 +3540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15">
       <c r="B4" s="73"/>
       <c r="C4" s="74"/>
       <c r="D4" s="74"/>
@@ -3471,7 +3556,7 @@
       <c r="N4" s="111"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="17" thickBot="1">
       <c r="B5" s="73"/>
       <c r="C5" s="20" t="s">
         <v>55</v>
@@ -3489,7 +3574,7 @@
       <c r="N5" s="16"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="17" thickBot="1">
       <c r="B6" s="73"/>
       <c r="C6" s="125" t="s">
         <v>38</v>
@@ -3515,7 +3600,7 @@
       <c r="N6" s="16"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B7" s="5"/>
       <c r="C7" s="126" t="s">
         <v>39</v>
@@ -3545,7 +3630,7 @@
       <c r="N7" s="16"/>
       <c r="O7" s="133"/>
     </row>
-    <row r="8" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="126" t="s">
         <v>82</v>
@@ -3575,7 +3660,7 @@
       <c r="N8" s="16"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="2:15" s="150" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" s="150" customFormat="1" ht="17" thickBot="1">
       <c r="B9" s="146"/>
       <c r="C9" s="147" t="s">
         <v>105</v>
@@ -3601,7 +3686,7 @@
       <c r="N9" s="16"/>
       <c r="O9" s="145"/>
     </row>
-    <row r="10" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B10" s="5"/>
       <c r="C10" s="127" t="s">
         <v>40</v>
@@ -3617,12 +3702,12 @@
       </c>
       <c r="G10" s="115">
         <f>I10</f>
-        <v>7.5499999999999998E-2</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="115">
         <f>Notes!F12</f>
-        <v>7.5499999999999998E-2</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -3631,7 +3716,7 @@
       <c r="N10" s="16"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15">
       <c r="B11" s="73"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -3647,7 +3732,7 @@
       <c r="N11" s="16"/>
       <c r="O11" s="133"/>
     </row>
-    <row r="12" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="17" thickBot="1">
       <c r="B12" s="73"/>
       <c r="C12" s="20" t="s">
         <v>37</v>
@@ -3665,7 +3750,7 @@
       <c r="N12" s="16"/>
       <c r="O12" s="133"/>
     </row>
-    <row r="13" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="17" thickBot="1">
       <c r="B13" s="73"/>
       <c r="C13" s="128" t="s">
         <v>43</v>
@@ -3693,7 +3778,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="17" thickBot="1">
       <c r="B14" s="73"/>
       <c r="C14" s="128" t="s">
         <v>44</v>
@@ -3721,7 +3806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="17" thickBot="1">
       <c r="B15" s="73"/>
       <c r="C15" s="128" t="s">
         <v>47</v>
@@ -3749,7 +3834,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="17" thickBot="1">
       <c r="B16" s="73"/>
       <c r="C16" s="128" t="s">
         <v>46</v>
@@ -3777,7 +3862,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="17" thickBot="1">
       <c r="B17" s="73"/>
       <c r="C17" s="128" t="s">
         <v>40</v>
@@ -3805,7 +3890,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="17" thickBot="1">
       <c r="B18" s="73"/>
       <c r="C18" s="128" t="s">
         <v>45</v>
@@ -3833,7 +3918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="17" thickBot="1">
       <c r="B19" s="84"/>
       <c r="C19" s="85"/>
       <c r="D19" s="85"/>
@@ -3849,22 +3934,22 @@
       <c r="N19" s="85"/>
       <c r="O19" s="86"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15">
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15">
       <c r="M21" s="18"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15">
       <c r="M22" s="18"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15">
       <c r="M23" s="18"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="M24" s="18"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15">
       <c r="O25" s="133"/>
     </row>
   </sheetData>
@@ -3874,17 +3959,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet4">
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B1:L14"/>
+  <dimension ref="B1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="49" customWidth="1"/>
     <col min="2" max="2" width="3.5" style="49" customWidth="1"/>
@@ -3899,8 +3984,8 @@
     <col min="13" max="16384" width="33.1640625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="17" thickBot="1"/>
+    <row r="2" spans="2:13">
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
@@ -3913,7 +3998,7 @@
       <c r="K2" s="53"/>
       <c r="L2" s="52"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13">
       <c r="B3" s="54"/>
       <c r="C3" s="55" t="s">
         <v>11</v>
@@ -3928,7 +4013,7 @@
       <c r="K3" s="56"/>
       <c r="L3" s="57"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13">
       <c r="B4" s="54"/>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
@@ -3941,7 +4026,7 @@
       <c r="K4" s="58"/>
       <c r="L4" s="57"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13">
       <c r="B5" s="59"/>
       <c r="C5" s="60" t="s">
         <v>13</v>
@@ -3970,7 +4055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13">
       <c r="B6" s="54"/>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
@@ -3983,7 +4068,7 @@
       <c r="K6" s="56"/>
       <c r="L6" s="55"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13">
       <c r="B7" s="54"/>
       <c r="C7" s="151" t="s">
         <v>82</v>
@@ -4010,7 +4095,7 @@
       </c>
       <c r="L7" s="63"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13">
       <c r="B8" s="54"/>
       <c r="C8" s="152" t="s">
         <v>77</v>
@@ -4018,7 +4103,7 @@
       <c r="E8" s="137"/>
       <c r="F8" s="137"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13">
       <c r="B9" s="54"/>
       <c r="C9" s="153" t="s">
         <v>40</v>
@@ -4026,13 +4111,13 @@
       <c r="E9" s="137"/>
       <c r="F9" s="137"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13">
       <c r="B10" s="54"/>
       <c r="C10" s="121"/>
       <c r="E10" s="137"/>
       <c r="F10" s="137"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13">
       <c r="B11" s="54"/>
       <c r="C11" s="62" t="s">
         <v>68</v>
@@ -4057,7 +4142,7 @@
       </c>
       <c r="L11" s="63"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13">
       <c r="B12" s="54"/>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
@@ -4070,7 +4155,7 @@
       <c r="K12" s="64"/>
       <c r="L12" s="63"/>
     </row>
-    <row r="13" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="21">
       <c r="B13" s="54"/>
       <c r="C13" s="62" t="s">
         <v>39</v>
@@ -4095,10 +4180,19 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13">
       <c r="B14" s="54"/>
       <c r="E14" s="137"/>
       <c r="F14" s="137"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="C15" s="153" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="M15" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4107,14 +4201,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Y154"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5.5" style="116" customWidth="1"/>
     <col min="2" max="2" width="5" style="116" customWidth="1"/>
@@ -4126,8 +4220,8 @@
     <col min="13" max="16384" width="7" style="116"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:25" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:25" ht="17" thickBot="1"/>
+    <row r="2" spans="2:25" s="26" customFormat="1">
       <c r="B2" s="119"/>
       <c r="C2" s="120" t="s">
         <v>25</v>
@@ -4155,7 +4249,7 @@
       <c r="T2" s="120"/>
       <c r="U2" s="120"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:25">
       <c r="B3" s="117"/>
       <c r="C3" s="118"/>
       <c r="D3" s="118"/>
@@ -4177,7 +4271,7 @@
       <c r="T3" s="118"/>
       <c r="U3" s="118"/>
     </row>
-    <row r="4" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:25" customFormat="1">
       <c r="B4" s="117"/>
       <c r="C4" s="129" t="s">
         <v>57</v>
@@ -4205,7 +4299,7 @@
       <c r="X4" s="129"/>
       <c r="Y4" s="129"/>
     </row>
-    <row r="5" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:25" customFormat="1">
       <c r="B5" s="117"/>
       <c r="C5" s="129"/>
       <c r="D5" s="129"/>
@@ -4231,7 +4325,7 @@
       <c r="X5" s="129"/>
       <c r="Y5" s="129"/>
     </row>
-    <row r="6" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:25" customFormat="1">
       <c r="B6" s="117"/>
       <c r="C6" s="129"/>
       <c r="D6" s="129"/>
@@ -4257,7 +4351,7 @@
       <c r="X6" s="129"/>
       <c r="Y6" s="129"/>
     </row>
-    <row r="7" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:25" customFormat="1">
       <c r="B7" s="117"/>
       <c r="C7" s="129"/>
       <c r="D7" s="129"/>
@@ -4283,7 +4377,7 @@
       <c r="X7" s="129"/>
       <c r="Y7" s="129"/>
     </row>
-    <row r="8" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:25" customFormat="1">
       <c r="B8" s="117"/>
       <c r="C8" s="129"/>
       <c r="D8" s="129">
@@ -4319,7 +4413,7 @@
       <c r="X8" s="129"/>
       <c r="Y8" s="129"/>
     </row>
-    <row r="9" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:25" customFormat="1">
       <c r="B9" s="117"/>
       <c r="C9" s="129"/>
       <c r="D9" s="129"/>
@@ -4350,7 +4444,7 @@
       <c r="X9" s="129"/>
       <c r="Y9" s="129"/>
     </row>
-    <row r="10" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:25" customFormat="1">
       <c r="B10" s="117"/>
       <c r="C10" s="129"/>
       <c r="D10" s="129"/>
@@ -4382,7 +4476,7 @@
       <c r="X10" s="129"/>
       <c r="Y10" s="129"/>
     </row>
-    <row r="11" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:25" customFormat="1">
       <c r="B11" s="117"/>
       <c r="C11" s="129"/>
       <c r="D11" s="129"/>
@@ -4414,13 +4508,13 @@
       <c r="X11" s="129"/>
       <c r="Y11" s="129"/>
     </row>
-    <row r="12" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:25" customFormat="1">
       <c r="B12" s="117"/>
       <c r="C12" s="129"/>
       <c r="D12" s="129"/>
       <c r="E12" s="129"/>
       <c r="F12" s="129">
-        <v>7.5499999999999998E-2</v>
+        <v>7.3300000000000004E-2</v>
       </c>
       <c r="G12" s="129" t="s">
         <v>72</v>
@@ -4430,7 +4524,9 @@
       </c>
       <c r="I12" s="129"/>
       <c r="J12" s="129"/>
-      <c r="K12" s="129"/>
+      <c r="K12" s="129" t="s">
+        <v>112</v>
+      </c>
       <c r="L12" s="129"/>
       <c r="M12" s="129"/>
       <c r="N12" s="129"/>
@@ -4446,7 +4542,7 @@
       <c r="X12" s="129"/>
       <c r="Y12" s="129"/>
     </row>
-    <row r="13" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:25" customFormat="1">
       <c r="B13" s="117"/>
       <c r="C13" s="129"/>
       <c r="D13" s="129"/>
@@ -4472,7 +4568,7 @@
       <c r="X13" s="129"/>
       <c r="Y13" s="129"/>
     </row>
-    <row r="14" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:25" customFormat="1">
       <c r="B14" s="117"/>
       <c r="C14" s="129"/>
       <c r="D14" s="129"/>
@@ -4498,7 +4594,7 @@
       <c r="X14" s="129"/>
       <c r="Y14" s="129"/>
     </row>
-    <row r="15" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:25" customFormat="1">
       <c r="B15" s="117"/>
       <c r="C15" s="129"/>
       <c r="D15" s="129"/>
@@ -4524,7 +4620,7 @@
       <c r="X15" s="129"/>
       <c r="Y15" s="129"/>
     </row>
-    <row r="16" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:25" customFormat="1">
       <c r="B16" s="117"/>
       <c r="C16" s="129"/>
       <c r="D16" s="129"/>
@@ -4550,7 +4646,7 @@
       <c r="X16" s="129"/>
       <c r="Y16" s="129"/>
     </row>
-    <row r="17" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:25" customFormat="1">
       <c r="B17" s="117"/>
       <c r="C17" s="129"/>
       <c r="D17" s="129"/>
@@ -4576,7 +4672,7 @@
       <c r="X17" s="129"/>
       <c r="Y17" s="129"/>
     </row>
-    <row r="18" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:25" customFormat="1">
       <c r="B18" s="117"/>
       <c r="C18" s="129"/>
       <c r="D18" s="129"/>
@@ -4602,7 +4698,7 @@
       <c r="X18" s="129"/>
       <c r="Y18" s="129"/>
     </row>
-    <row r="19" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:25" customFormat="1">
       <c r="B19" s="117"/>
       <c r="C19" s="129"/>
       <c r="D19" s="129"/>
@@ -4628,7 +4724,7 @@
       <c r="X19" s="129"/>
       <c r="Y19" s="129"/>
     </row>
-    <row r="20" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:25" customFormat="1">
       <c r="B20" s="117"/>
       <c r="C20" s="129"/>
       <c r="D20" s="129"/>
@@ -4654,7 +4750,7 @@
       <c r="X20" s="129"/>
       <c r="Y20" s="129"/>
     </row>
-    <row r="21" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:25" customFormat="1">
       <c r="B21" s="117"/>
       <c r="C21" s="129"/>
       <c r="D21" s="129"/>
@@ -4680,7 +4776,7 @@
       <c r="X21" s="129"/>
       <c r="Y21" s="129"/>
     </row>
-    <row r="22" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:25" customFormat="1">
       <c r="B22" s="117"/>
       <c r="C22" s="129"/>
       <c r="D22" s="129"/>
@@ -4706,7 +4802,7 @@
       <c r="X22" s="129"/>
       <c r="Y22" s="129"/>
     </row>
-    <row r="23" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:25" customFormat="1">
       <c r="B23" s="117"/>
       <c r="C23" s="129"/>
       <c r="D23" s="129"/>
@@ -4732,7 +4828,7 @@
       <c r="X23" s="129"/>
       <c r="Y23" s="129"/>
     </row>
-    <row r="24" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:25" customFormat="1">
       <c r="B24" s="117"/>
       <c r="C24" s="129"/>
       <c r="D24" s="129"/>
@@ -4758,7 +4854,7 @@
       <c r="X24" s="129"/>
       <c r="Y24" s="129"/>
     </row>
-    <row r="25" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:25" customFormat="1">
       <c r="B25" s="117"/>
       <c r="C25" s="129"/>
       <c r="D25" s="129"/>
@@ -4784,7 +4880,7 @@
       <c r="X25" s="129"/>
       <c r="Y25" s="129"/>
     </row>
-    <row r="26" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:25" customFormat="1">
       <c r="B26" s="117"/>
       <c r="C26" s="129"/>
       <c r="D26" s="129"/>
@@ -4810,7 +4906,7 @@
       <c r="X26" s="129"/>
       <c r="Y26" s="129"/>
     </row>
-    <row r="27" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:25" customFormat="1">
       <c r="B27" s="117"/>
       <c r="C27" s="129"/>
       <c r="D27" s="129"/>
@@ -4836,7 +4932,7 @@
       <c r="X27" s="129"/>
       <c r="Y27" s="129"/>
     </row>
-    <row r="28" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:25" customFormat="1">
       <c r="B28" s="117"/>
       <c r="C28" s="129"/>
       <c r="D28" s="129"/>
@@ -4862,106 +4958,112 @@
       <c r="X28" s="129"/>
       <c r="Y28" s="129"/>
     </row>
-    <row r="29" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:25" customFormat="1">
       <c r="B29" s="117"/>
     </row>
-    <row r="30" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:25" customFormat="1">
       <c r="B30" s="117"/>
     </row>
-    <row r="31" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:25" customFormat="1">
       <c r="B31" s="117"/>
     </row>
-    <row r="32" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:25" customFormat="1">
       <c r="B32" s="117"/>
     </row>
-    <row r="33" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" customFormat="1">
       <c r="B33" s="117"/>
     </row>
-    <row r="34" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" customFormat="1">
       <c r="B34" s="117"/>
     </row>
-    <row r="35" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" customFormat="1">
       <c r="B35" s="117"/>
     </row>
-    <row r="36" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" customFormat="1">
       <c r="B36" s="117"/>
     </row>
-    <row r="37" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" customFormat="1">
       <c r="B37" s="117"/>
     </row>
-    <row r="38" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" customFormat="1">
       <c r="B38" s="117"/>
     </row>
-    <row r="39" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" customFormat="1">
       <c r="B39" s="117"/>
     </row>
-    <row r="40" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" customFormat="1">
       <c r="B40" s="117"/>
     </row>
-    <row r="41" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" customFormat="1">
       <c r="B41" s="117"/>
     </row>
-    <row r="42" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" customFormat="1">
       <c r="B42" s="117"/>
     </row>
-    <row r="43" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" customFormat="1">
       <c r="B43" s="117"/>
     </row>
-    <row r="44" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" customFormat="1">
       <c r="B44" s="117"/>
     </row>
-    <row r="45" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" customFormat="1">
       <c r="B45" s="117"/>
     </row>
-    <row r="46" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" customFormat="1">
       <c r="B46" s="117"/>
     </row>
-    <row r="47" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" customFormat="1">
       <c r="B47" s="117"/>
     </row>
-    <row r="48" spans="2:2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" customFormat="1">
       <c r="B48" s="117"/>
     </row>
-    <row r="49" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" customFormat="1">
       <c r="B49" s="117"/>
     </row>
-    <row r="50" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" customFormat="1">
       <c r="B50" s="117"/>
     </row>
-    <row r="51" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" customFormat="1">
       <c r="B51" s="117"/>
-    </row>
-    <row r="52" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" customFormat="1">
       <c r="B52" s="117"/>
     </row>
-    <row r="53" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" customFormat="1">
       <c r="B53" s="117"/>
-    </row>
-    <row r="54" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" customFormat="1">
       <c r="B54" s="117"/>
     </row>
-    <row r="55" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" customFormat="1">
       <c r="B55" s="117"/>
     </row>
-    <row r="56" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" customFormat="1">
       <c r="B56" s="117"/>
     </row>
-    <row r="57" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" customFormat="1">
       <c r="B57" s="117"/>
     </row>
-    <row r="58" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" customFormat="1">
       <c r="B58" s="117"/>
     </row>
-    <row r="59" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" customFormat="1">
       <c r="B59" s="117"/>
     </row>
-    <row r="60" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" customFormat="1">
       <c r="B60" s="117"/>
     </row>
-    <row r="61" spans="1:25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" customFormat="1" ht="17" thickBot="1">
       <c r="B61" s="117"/>
     </row>
-    <row r="62" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" s="26" customFormat="1">
       <c r="A62"/>
       <c r="B62" s="119"/>
       <c r="C62" s="120" t="s">
@@ -4990,7 +5092,7 @@
       <c r="T62" s="120"/>
       <c r="U62" s="120"/>
     </row>
-    <row r="63" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" customFormat="1">
       <c r="B63" s="117"/>
       <c r="C63" s="132"/>
       <c r="D63" s="129"/>
@@ -5016,7 +5118,7 @@
       <c r="X63" s="129"/>
       <c r="Y63" s="129"/>
     </row>
-    <row r="64" spans="1:25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" customFormat="1" ht="21">
       <c r="B64" s="117"/>
       <c r="C64" s="138" t="s">
         <v>67</v>
@@ -5044,7 +5146,7 @@
       <c r="X64" s="129"/>
       <c r="Y64" s="129"/>
     </row>
-    <row r="65" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:25" customFormat="1">
       <c r="B65" s="117"/>
       <c r="C65" s="129"/>
       <c r="D65" s="129"/>
@@ -5070,7 +5172,7 @@
       <c r="X65" s="129"/>
       <c r="Y65" s="129"/>
     </row>
-    <row r="66" spans="2:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:25" customFormat="1">
       <c r="B66" s="117"/>
       <c r="C66" s="129"/>
       <c r="D66" s="129"/>
@@ -5096,17 +5198,17 @@
       <c r="X66" s="129"/>
       <c r="Y66" s="129"/>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:25">
       <c r="D68" s="116">
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:25">
       <c r="E73" s="139" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:25">
       <c r="E74" s="129" t="s">
         <v>43</v>
       </c>
@@ -5123,7 +5225,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:25">
       <c r="E75" s="129" t="s">
         <v>44</v>
       </c>
@@ -5138,7 +5240,7 @@
       <c r="J75" s="129"/>
       <c r="K75" s="129"/>
     </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:25">
       <c r="E76" s="129" t="s">
         <v>47</v>
       </c>
@@ -5153,7 +5255,7 @@
       <c r="J76" s="129"/>
       <c r="K76" s="129"/>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:25">
       <c r="D77" s="129"/>
       <c r="E77" s="129" t="s">
         <v>46</v>
@@ -5169,7 +5271,7 @@
       <c r="J77" s="129"/>
       <c r="K77" s="129"/>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:25">
       <c r="D78" s="129"/>
       <c r="E78" s="129" t="s">
         <v>40</v>
@@ -5185,7 +5287,7 @@
       <c r="J78" s="129"/>
       <c r="K78" s="129"/>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:25">
       <c r="D79" s="129"/>
       <c r="E79" s="129" t="s">
         <v>45</v>
@@ -5203,7 +5305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:25">
       <c r="D80" s="129"/>
       <c r="E80" s="129"/>
       <c r="F80" s="129"/>
@@ -5212,7 +5314,7 @@
       <c r="I80" s="129"/>
       <c r="J80" s="129"/>
     </row>
-    <row r="81" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:11">
       <c r="D81" s="129"/>
       <c r="E81" s="129"/>
       <c r="F81" s="129"/>
@@ -5221,7 +5323,7 @@
       <c r="I81" s="129"/>
       <c r="J81" s="129"/>
     </row>
-    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:11">
       <c r="D82" s="129"/>
       <c r="E82" s="129" t="s">
         <v>43</v>
@@ -5240,7 +5342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:11">
       <c r="E83" s="129" t="s">
         <v>44</v>
       </c>
@@ -5256,7 +5358,7 @@
       <c r="J83" s="129"/>
       <c r="K83" s="129"/>
     </row>
-    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:11">
       <c r="E84" s="129" t="s">
         <v>47</v>
       </c>
@@ -5272,7 +5374,7 @@
       <c r="J84" s="129"/>
       <c r="K84" s="129"/>
     </row>
-    <row r="85" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:11">
       <c r="E85" s="129" t="s">
         <v>46</v>
       </c>
@@ -5288,7 +5390,7 @@
       <c r="J85" s="129"/>
       <c r="K85" s="129"/>
     </row>
-    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:11">
       <c r="E86" s="129" t="s">
         <v>40</v>
       </c>
@@ -5304,7 +5406,7 @@
       <c r="J86" s="129"/>
       <c r="K86" s="129"/>
     </row>
-    <row r="87" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:11">
       <c r="E87" s="129" t="s">
         <v>45</v>
       </c>
@@ -5322,7 +5424,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:11">
       <c r="E90" s="140"/>
       <c r="F90" s="141"/>
       <c r="G90" s="141"/>
@@ -5331,7 +5433,7 @@
       <c r="J90" s="141"/>
       <c r="K90" s="141"/>
     </row>
-    <row r="91" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:11">
       <c r="E91" s="129"/>
       <c r="F91" s="129"/>
       <c r="G91" s="129"/>
@@ -5340,7 +5442,7 @@
       <c r="J91" s="129"/>
       <c r="K91" s="129"/>
     </row>
-    <row r="92" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:11">
       <c r="E92" s="129"/>
       <c r="F92" s="129"/>
       <c r="G92" s="129"/>
@@ -5349,7 +5451,7 @@
       <c r="J92" s="129"/>
       <c r="K92" s="129"/>
     </row>
-    <row r="93" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:11">
       <c r="E93" s="129"/>
       <c r="F93" s="129"/>
       <c r="G93" s="129"/>
@@ -5358,7 +5460,7 @@
       <c r="J93" s="129"/>
       <c r="K93" s="129"/>
     </row>
-    <row r="94" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:11">
       <c r="E94" s="129"/>
       <c r="F94" s="129"/>
       <c r="G94" s="129"/>
@@ -5367,7 +5469,7 @@
       <c r="J94" s="129"/>
       <c r="K94" s="129"/>
     </row>
-    <row r="95" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:11">
       <c r="E95" s="129"/>
       <c r="F95" s="129"/>
       <c r="G95" s="129"/>
@@ -5376,7 +5478,7 @@
       <c r="J95" s="129"/>
       <c r="K95" s="129"/>
     </row>
-    <row r="96" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:11">
       <c r="E96" s="129"/>
       <c r="F96" s="129"/>
       <c r="G96" s="129"/>
@@ -5385,7 +5487,7 @@
       <c r="J96" s="129"/>
       <c r="K96" s="129"/>
     </row>
-    <row r="97" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:11">
       <c r="E97" s="129"/>
       <c r="F97" s="129"/>
       <c r="G97" s="129"/>
@@ -5394,7 +5496,7 @@
       <c r="J97" s="129"/>
       <c r="K97" s="141"/>
     </row>
-    <row r="98" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:11">
       <c r="E98" s="129"/>
       <c r="F98" s="129"/>
       <c r="G98" s="129"/>
@@ -5403,7 +5505,7 @@
       <c r="J98" s="129"/>
       <c r="K98" s="141"/>
     </row>
-    <row r="99" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:11">
       <c r="E99" s="129"/>
       <c r="F99" s="129"/>
       <c r="G99" s="129"/>
@@ -5412,7 +5514,7 @@
       <c r="J99" s="129"/>
       <c r="K99" s="129"/>
     </row>
-    <row r="100" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:11">
       <c r="E100" s="129"/>
       <c r="F100" s="129"/>
       <c r="G100" s="129"/>
@@ -5421,7 +5523,7 @@
       <c r="J100" s="129"/>
       <c r="K100" s="129"/>
     </row>
-    <row r="101" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:11">
       <c r="E101" s="129"/>
       <c r="F101" s="129"/>
       <c r="G101" s="129"/>
@@ -5430,7 +5532,7 @@
       <c r="J101" s="129"/>
       <c r="K101" s="129"/>
     </row>
-    <row r="102" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:11">
       <c r="E102" s="129"/>
       <c r="F102" s="129"/>
       <c r="G102" s="129"/>
@@ -5439,7 +5541,7 @@
       <c r="J102" s="129"/>
       <c r="K102" s="129"/>
     </row>
-    <row r="103" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:11">
       <c r="E103" s="129"/>
       <c r="F103" s="129"/>
       <c r="G103" s="129"/>
@@ -5448,7 +5550,7 @@
       <c r="J103" s="129"/>
       <c r="K103" s="129"/>
     </row>
-    <row r="104" spans="5:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:11">
       <c r="E104" s="129"/>
       <c r="F104" s="129"/>
       <c r="G104" s="129"/>
@@ -5457,9 +5559,9 @@
       <c r="J104" s="129"/>
       <c r="K104" s="129"/>
     </row>
-    <row r="122" spans="1:25" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" spans="1:25" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:25" customFormat="1"/>
+    <row r="123" spans="1:25" customFormat="1" ht="17" thickBot="1"/>
+    <row r="124" spans="1:25" s="26" customFormat="1">
       <c r="A124"/>
       <c r="B124" s="119"/>
       <c r="C124" s="120" t="s">
@@ -5488,7 +5590,7 @@
       <c r="T124" s="120"/>
       <c r="U124" s="120"/>
     </row>
-    <row r="125" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:25" customFormat="1">
       <c r="B125" s="117"/>
       <c r="C125" s="132"/>
       <c r="D125" s="129"/>
@@ -5514,7 +5616,7 @@
       <c r="X125" s="129"/>
       <c r="Y125" s="129"/>
     </row>
-    <row r="126" spans="1:25" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" customFormat="1" ht="21">
       <c r="B126" s="117"/>
       <c r="C126" s="138" t="s">
         <v>96</v>
@@ -5542,7 +5644,7 @@
       <c r="X126" s="129"/>
       <c r="Y126" s="129"/>
     </row>
-    <row r="127" spans="1:25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:25" customFormat="1">
       <c r="B127" s="117"/>
       <c r="C127" s="129"/>
       <c r="D127" s="129"/>
@@ -5568,13 +5670,13 @@
       <c r="X127" s="129"/>
       <c r="Y127" s="129"/>
     </row>
-    <row r="128" spans="1:25" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" spans="6:17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:25" customFormat="1"/>
+    <row r="129" spans="6:17" customFormat="1">
       <c r="F129" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="130" spans="6:17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="6:17" customFormat="1">
       <c r="L130" s="173" t="s">
         <v>87</v>
       </c>
@@ -5594,7 +5696,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="131" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="131" spans="6:17">
       <c r="G131" s="116">
         <f>AVERAGE(P131:P152)</f>
         <v>45.192272727272723</v>
@@ -5624,7 +5726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="132" spans="6:17">
       <c r="G132" s="116">
         <v>158.98729499999999</v>
       </c>
@@ -5650,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="133" spans="6:17">
       <c r="G133" s="116">
         <f>G131/litres_per_barrel</f>
         <v>0.28425084361157743</v>
@@ -5677,7 +5779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="134" spans="6:17">
       <c r="G134" s="116">
         <f>dollar_per_euro</f>
         <v>1.1718999999999999</v>
@@ -5704,7 +5806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="135" spans="6:17">
       <c r="G135" s="116">
         <f>G133/G134</f>
         <v>0.24255554536357832</v>
@@ -5731,7 +5833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="136" spans="6:17">
       <c r="G136" s="116">
         <f>F11</f>
         <v>34.44</v>
@@ -5758,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="137" spans="6:17">
       <c r="G137" s="167">
         <f>G135/G136</f>
         <v>7.0428439420318909E-3</v>
@@ -5785,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="138" spans="6:17">
       <c r="L138" s="182">
         <v>42907</v>
       </c>
@@ -5805,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="139" spans="6:17">
       <c r="L139" s="182">
         <v>42906</v>
       </c>
@@ -5825,7 +5927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="140" spans="6:17">
       <c r="L140" s="182">
         <v>42905</v>
       </c>
@@ -5845,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="141" spans="6:17">
       <c r="L141" s="182">
         <v>42902</v>
       </c>
@@ -5865,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="142" spans="6:17">
       <c r="L142" s="182">
         <v>42901</v>
       </c>
@@ -5885,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="143" spans="6:17">
       <c r="L143" s="182">
         <v>42900</v>
       </c>
@@ -5905,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="6:17" x14ac:dyDescent="0.2">
+    <row r="144" spans="6:17">
       <c r="L144" s="182">
         <v>42899</v>
       </c>
@@ -5925,7 +6027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="145" spans="12:17">
       <c r="L145" s="182">
         <v>42898</v>
       </c>
@@ -5945,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="146" spans="12:17">
       <c r="L146" s="182">
         <v>42895</v>
       </c>
@@ -5965,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="147" spans="12:17">
       <c r="L147" s="182">
         <v>42894</v>
       </c>
@@ -5985,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="148" spans="12:17">
       <c r="L148" s="182">
         <v>42893</v>
       </c>
@@ -6005,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="149" spans="12:17">
       <c r="L149" s="182">
         <v>42892</v>
       </c>
@@ -6025,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="150" spans="12:17">
       <c r="L150" s="182">
         <v>42891</v>
       </c>
@@ -6045,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="151" spans="12:17">
       <c r="L151" s="182">
         <v>42888</v>
       </c>
@@ -6065,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="152" spans="12:17">
       <c r="L152" s="182">
         <v>42887</v>
       </c>
@@ -6085,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="153" spans="12:17">
       <c r="L153" s="174"/>
       <c r="M153" s="173"/>
       <c r="N153" s="173"/>
@@ -6093,7 +6195,7 @@
       <c r="P153" s="173"/>
       <c r="Q153" s="173"/>
     </row>
-    <row r="154" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="154" spans="12:17">
       <c r="L154" s="174"/>
       <c r="M154" s="173"/>
       <c r="N154" s="173"/>
@@ -6109,14 +6211,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="3.33203125" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
@@ -6127,13 +6229,13 @@
     <col min="9" max="9" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="161" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" s="161" customFormat="1">
       <c r="D1" s="162"/>
       <c r="E1" s="162"/>
       <c r="F1" s="162"/>
       <c r="G1" s="162"/>
     </row>
-    <row r="2" spans="2:9" s="161" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" s="161" customFormat="1" ht="15" customHeight="1">
       <c r="B2" s="183" t="s">
         <v>85</v>
       </c>
@@ -6143,7 +6245,7 @@
       <c r="F2" s="162"/>
       <c r="G2" s="162"/>
     </row>
-    <row r="3" spans="2:9" s="161" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" s="161" customFormat="1">
       <c r="B3" s="186"/>
       <c r="C3" s="187"/>
       <c r="D3" s="187"/>
@@ -6151,7 +6253,7 @@
       <c r="F3" s="162"/>
       <c r="G3" s="162"/>
     </row>
-    <row r="4" spans="2:9" s="161" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" s="161" customFormat="1">
       <c r="B4" s="189"/>
       <c r="C4" s="190"/>
       <c r="D4" s="190"/>
@@ -6159,10 +6261,10 @@
       <c r="F4" s="162"/>
       <c r="G4" s="162"/>
     </row>
-    <row r="5" spans="2:9" s="161" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" s="161" customFormat="1" ht="17" thickBot="1">
       <c r="D5" s="162"/>
     </row>
-    <row r="6" spans="2:9" s="161" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" s="161" customFormat="1">
       <c r="B6" s="163"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -6172,7 +6274,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="164"/>
     </row>
-    <row r="7" spans="2:9" s="45" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" s="45" customFormat="1" ht="19">
       <c r="B7" s="103"/>
       <c r="C7" s="21" t="s">
         <v>86</v>
@@ -6194,11 +6296,11 @@
       </c>
       <c r="I7" s="107"/>
     </row>
-    <row r="8" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" ht="20" thickBot="1">
       <c r="B8" s="25"/>
       <c r="I8" s="46"/>
     </row>
-    <row r="9" spans="2:9" s="45" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="25"/>
       <c r="C9" s="165" t="s">
         <v>88</v>

</xml_diff>